<commit_message>
add base url on supabase env
</commit_message>
<xml_diff>
--- a/seeds/schemas/tenant_accounts.xlsx
+++ b/seeds/schemas/tenant_accounts.xlsx
@@ -5,15 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns_mapper" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="navigation_bar" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="navigation_bar_item" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="role" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="user" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="navigation_bar" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="navigation_bar_item" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">navigation_bar_item!$A$1:$D$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">navigation_bar_item!$A$1:$D$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -81,34 +83,64 @@
     <t xml:space="preserve">partial_type_id**tenants_schema.partial_type**partial_type_name</t>
   </si>
   <si>
+    <t xml:space="preserve">role_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role_security_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc moderator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenant moderator role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TenantFind|TenantList|TenantUpdate|PageFind|PageList|PageUpdate|SectionFind|SectionList|SectionUpdate|PartialList|PartialCreate|PartialUpdate|PartialDelete|PartialDeleteRestore|FileList|FileUpdate|FileCreate|FileDelete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech Innovators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user_password#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heba@abchotels-eg.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC Hotels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rashad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rashad@abchotels-eg.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">navigation_bar_name</t>
   </si>
   <si>
     <t xml:space="preserve">abchotels_header</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC Hotels</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">abchotels_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">footer</t>
-    </r>
+    <t xml:space="preserve">abchotels_footer</t>
   </si>
   <si>
     <t xml:space="preserve">menu_key</t>
@@ -132,41 +164,13 @@
     <t xml:space="preserve">الرئيسية</t>
   </si>
   <si>
-    <t xml:space="preserve">/home</t>
+    <t xml:space="preserve">/landing</t>
   </si>
   <si>
     <t xml:space="preserve">null</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">02_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">header_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">about</t>
-    </r>
+    <t xml:space="preserve">02_header_about</t>
   </si>
   <si>
     <t xml:space="preserve">About Us</t>
@@ -178,35 +182,7 @@
     <t xml:space="preserve">/about</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">03_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">header_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">services</t>
-    </r>
+    <t xml:space="preserve">03_header_services</t>
   </si>
   <si>
     <t xml:space="preserve">Services</t>
@@ -221,35 +197,7 @@
     <t xml:space="preserve">service</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">04_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">header_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">projects</t>
-    </r>
+    <t xml:space="preserve">04_header_projects</t>
   </si>
   <si>
     <t xml:space="preserve">Projects</t>
@@ -280,46 +228,7 @@
         <color theme="1"/>
         <rFont val="CommitMono Nerd Font"/>
         <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">header_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
         <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">gallery</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">الاستوديو</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/gallery</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">06_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="CommitMono Nerd Font"/>
-        <family val="0"/>
       </rPr>
       <t xml:space="preserve">header_</t>
     </r>
@@ -335,7 +244,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Contact</t>
+    <t xml:space="preserve">Contact Us</t>
   </si>
   <si>
     <t xml:space="preserve">اتصل بنا</t>
@@ -356,6 +265,12 @@
     <t xml:space="preserve">Our Gallery</t>
   </si>
   <si>
+    <t xml:space="preserve">الاستوديو</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/gallery</t>
+  </si>
+  <si>
     <t xml:space="preserve">03_footer_services</t>
   </si>
   <si>
@@ -375,9 +290,6 @@
   </si>
   <si>
     <t xml:space="preserve">05_footer_contact_us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Us</t>
   </si>
 </sst>
 </file>
@@ -387,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,16 +330,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="CommitMono Nerd Font"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -492,7 +398,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,7 +420,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -526,14 +432,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -761,7 +659,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="98.16"/>
@@ -832,10 +730,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -855,41 +753,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q44" activeCellId="0" sqref="Q44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.81"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+    <row r="2" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -906,34 +817,187 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="77.515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1020002001</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1020002002</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="heba@abchotels-eg.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="rashad@abchotels-eg.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.81"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="18.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="57.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -947,288 +1011,252 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>34</v>
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="39.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>60</v>
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>21</v>
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="10"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D4"/>
+  <autoFilter ref="A1:D3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>